<commit_message>
Vol of vol plot
</commit_message>
<xml_diff>
--- a/Artifacts/FwdVarSwapRollDown.xlsx
+++ b/Artifacts/FwdVarSwapRollDown.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="24700" windowHeight="15360" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="7260" yWindow="0" windowWidth="24980" windowHeight="15600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PureFwdStart" sheetId="1" r:id="rId1"/>
@@ -178,7 +178,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -848,11 +847,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2094749576"/>
-        <c:axId val="-2094754536"/>
+        <c:axId val="-2089845864"/>
+        <c:axId val="-2030130744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2094749576"/>
+        <c:axId val="-2089845864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -862,7 +861,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2094754536"/>
+        <c:crossAx val="-2030130744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -870,7 +869,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2094754536"/>
+        <c:axId val="-2030130744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -881,14 +880,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2094749576"/>
+        <c:crossAx val="-2089845864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1040,11 +1038,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2097068360"/>
-        <c:axId val="-2097148760"/>
+        <c:axId val="-2043448520"/>
+        <c:axId val="-2115000184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2097068360"/>
+        <c:axId val="-2043448520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1053,7 +1051,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2097148760"/>
+        <c:crossAx val="-2115000184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1061,7 +1059,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2097148760"/>
+        <c:axId val="-2115000184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1072,7 +1070,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2097068360"/>
+        <c:crossAx val="-2043448520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3348,7 +3346,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F32"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>